<commit_message>
Updated To Larger version work from tonight
Created a zip of the code and sent to sean and mick.
Finsished results.
Backed up data for gui.
Started discussion.
added in data to apendices.
added in notes what to talk about.
going well! :)
</commit_message>
<xml_diff>
--- a/Final Paper/Comparison Table 2.xlsx
+++ b/Final Paper/Comparison Table 2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c07c9239cf8ef362/4th Year Sem2/EG4012/Matlab GUI Thesis/Matlab-GUI-Thesis/Final Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="5156BC689B060479E16BCBAFF2AF9FBB13E03353" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{B506E686-5B47-48F3-A4BA-018426C0BA51}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16888" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16888" uniqueCount="185">
   <si>
     <t>HELP</t>
   </si>
@@ -540,7 +541,58 @@
     <t>Output Finance Figures</t>
   </si>
   <si>
-    <t xml:space="preserve">Net Present Value </t>
+    <t>Daily Usage (kWhr)</t>
+  </si>
+  <si>
+    <t>Daily Production (kWhr)</t>
+  </si>
+  <si>
+    <t>Daily Storage (kWhr)</t>
+  </si>
+  <si>
+    <t>Total Exported (kWhr)</t>
+  </si>
+  <si>
+    <t>Daily Cost – Standard ($AUD)</t>
+  </si>
+  <si>
+    <t>Daily Cost – Import ($AUD)</t>
+  </si>
+  <si>
+    <t>Daily Cost – Export ($AUD)</t>
+  </si>
+  <si>
+    <t>Daily Cost - Acutal Savings ($AUD)</t>
+  </si>
+  <si>
+    <t>Annualised Life Cycle Cost ($/kWhr)</t>
+  </si>
+  <si>
+    <t>Annual Payment -  Optimistic ($/kWhr)</t>
+  </si>
+  <si>
+    <t>Annual Payment -  Likely ($/kWhr)</t>
+  </si>
+  <si>
+    <t>Annual Payment -  Pessimistic ($/kWhr)</t>
+  </si>
+  <si>
+    <t>Expected Savings – Monthly ($AUD)</t>
+  </si>
+  <si>
+    <t>Expected Savings – Yearly ($AUD)</t>
+  </si>
+  <si>
+    <t>Expected Savings - 10 Year Period ($AUD)</t>
+  </si>
+  <si>
+    <t>Expected Savings - 20 Year Period ($AUD)</t>
+  </si>
+  <si>
+    <t>Payback Period (years)</t>
+  </si>
+  <si>
+    <t>Net Present Value ($AUD)</t>
   </si>
 </sst>
 </file>
@@ -1336,209 +1388,6 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1942,6 +1791,209 @@
       </font>
     </dxf>
     <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <color theme="1"/>
@@ -2084,43 +2136,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64F0368C-A621-4094-9DFE-ECE20E19140E}" name="Table134234" displayName="Table134234" ref="A3:F144" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{64F0368C-A621-4094-9DFE-ECE20E19140E}" name="Table134234" displayName="Table134234" ref="A3:F144" headerRowDxfId="35" dataDxfId="34">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{DCF214CF-4DCB-4F8A-85C4-BC1A7DAF2C3A}" name="FEATURES" totalsRowLabel="Total" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{4FDA35BD-BFB6-4494-8228-2A2E0CDDD289}" name="The Solar Solution" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{FEAA5A23-B897-4F32-A233-F59CEE9D0043}" name="Solar Choice" dataDxfId="5" totalsRowDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{8D98A8DC-B3E4-4316-8103-7D1D082601F3}" name="Solar Power Calculator" dataDxfId="3" totalsRowDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{EEAD0DA8-C97D-4805-8DA2-BCD305A89043}" name="Solar Savings" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{AB348F1E-34D2-4FA9-B9FF-CC290D8E7AAB}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{DCF214CF-4DCB-4F8A-85C4-BC1A7DAF2C3A}" name="FEATURES" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{4FDA35BD-BFB6-4494-8228-2A2E0CDDD289}" name="The Solar Solution" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{FEAA5A23-B897-4F32-A233-F59CEE9D0043}" name="Solar Choice" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{8D98A8DC-B3E4-4316-8103-7D1D082601F3}" name="Solar Power Calculator" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{EEAD0DA8-C97D-4805-8DA2-BCD305A89043}" name="Solar Savings" totalsRowFunction="count" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{AB348F1E-34D2-4FA9-B9FF-CC290D8E7AAB}" name="Column1" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DEA80E19-B115-4056-88DE-52944BD49752}" name="Table13423" displayName="Table13423" ref="A3:E45" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DEA80E19-B115-4056-88DE-52944BD49752}" name="Table13423" displayName="Table13423" ref="A3:E45" headerRowDxfId="23" dataDxfId="22">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{902D8989-BA26-429C-8D63-84F54D729967}" name="FEATURES" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{10A355FE-7D1F-49B0-8ACA-1B9A14C72955}" name="The Solar Solution" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{148D7756-D0DF-4232-8C7E-D44796A7E4AD}" name="Solar Power Calculator" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{F31549BA-163B-4D40-BB3A-77F2D7DAEB14}" name="Solar Choice" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{E4C89B09-62DD-43F3-ABCE-119443F63E34}" name="Solar Savings" totalsRowFunction="count" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{902D8989-BA26-429C-8D63-84F54D729967}" name="FEATURES" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{10A355FE-7D1F-49B0-8ACA-1B9A14C72955}" name="The Solar Solution" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{148D7756-D0DF-4232-8C7E-D44796A7E4AD}" name="Solar Power Calculator" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{F31549BA-163B-4D40-BB3A-77F2D7DAEB14}" name="Solar Choice" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{E4C89B09-62DD-43F3-ABCE-119443F63E34}" name="Solar Savings" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1342" displayName="Table1342" ref="A3:G26" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1342" displayName="Table1342" ref="A3:G26" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A3:G26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FEATURES" totalsRowLabel="Total" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PRODUCT NAME 1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PRODUCT NAME 2" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PRODUCT NAME 3" dataDxfId="17" totalsRowDxfId="16" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PRODUCT NAME 4" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PRODUCT NAME 5" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="PRODUCT NAME 6" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FEATURES" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PRODUCT NAME 1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PRODUCT NAME 2" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PRODUCT NAME 3" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PRODUCT NAME 4" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="PRODUCT NAME 5" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="PRODUCT NAME 6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -2394,8 +2446,8 @@
   </sheetPr>
   <dimension ref="A1:XFD145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3510,7 +3562,7 @@
     </row>
     <row r="43" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="108" t="s">
-        <v>101</v>
+        <v>167</v>
       </c>
       <c r="B43" s="118">
         <v>19.2</v>
@@ -3527,7 +3579,7 @@
     </row>
     <row r="44" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="108" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="B44" s="118">
         <v>24.692499999999999</v>
@@ -3544,7 +3596,7 @@
     </row>
     <row r="45" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="108" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="B45" s="118">
         <v>10</v>
@@ -3561,7 +3613,7 @@
     </row>
     <row r="46" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="108" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="B46" s="118">
         <v>6.4617000000000004</v>
@@ -3578,7 +3630,7 @@
     </row>
     <row r="47" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="108" t="s">
-        <v>136</v>
+        <v>171</v>
       </c>
       <c r="B47" s="118">
         <v>5.3261000000000003</v>
@@ -3595,7 +3647,7 @@
     </row>
     <row r="48" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="108" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="B48" s="118">
         <v>0.26879999999999998</v>
@@ -3612,7 +3664,7 @@
     </row>
     <row r="49" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="108" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="B49" s="118">
         <v>0.50009999999999999</v>
@@ -3629,7 +3681,7 @@
     </row>
     <row r="50" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="108" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="B50" s="118">
         <v>5.5574000000000003</v>
@@ -52878,7 +52930,7 @@
     </row>
     <row r="58" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="108" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="B58" s="118">
         <v>0.1603</v>
@@ -52895,7 +52947,7 @@
     </row>
     <row r="59" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="108" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="B59" s="118">
         <v>0.1623</v>
@@ -52912,7 +52964,7 @@
     </row>
     <row r="60" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="108" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="B60" s="118">
         <v>0.20610000000000001</v>
@@ -52929,7 +52981,7 @@
     </row>
     <row r="61" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="108" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="B61" s="118">
         <v>0.25540000000000002</v>
@@ -52980,7 +53032,7 @@
     </row>
     <row r="64" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="108" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
       <c r="B64" s="118">
         <v>166.721</v>
@@ -52997,7 +53049,7 @@
     </row>
     <row r="65" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="108" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="B65" s="118">
         <v>2028.4</v>
@@ -53014,7 +53066,7 @@
     </row>
     <row r="66" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="108" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="B66" s="118">
         <v>20284</v>
@@ -53031,7 +53083,7 @@
     </row>
     <row r="67" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="108" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="B67" s="118">
         <v>40569</v>
@@ -53048,7 +53100,7 @@
     </row>
     <row r="68" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="108" t="s">
-        <v>109</v>
+        <v>183</v>
       </c>
       <c r="B68" s="118">
         <v>13.014900000000001</v>
@@ -53065,7 +53117,7 @@
     </row>
     <row r="69" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="108" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B69" s="118">
         <v>16682</v>

</xml_diff>

<commit_message>
Working more on discussion
Dude i sooo need to code ... lol
</commit_message>
<xml_diff>
--- a/Final Paper/Comparison Table 2.xlsx
+++ b/Final Paper/Comparison Table 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c07c9239cf8ef362/4th Year Sem2/EG4012/Matlab GUI Thesis/Matlab-GUI-Thesis/Final Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="5156BC689B060479E16BCBAFF2AF9FBB13E03353" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{B506E686-5B47-48F3-A4BA-018426C0BA51}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="5156BC689B060479E16BCBAFF2AF9FBB13E03353" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{5FA85E99-6EBA-407A-9034-861FB4919556}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16888" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16893" uniqueCount="188">
   <si>
     <t>HELP</t>
   </si>
@@ -594,15 +594,25 @@
   <si>
     <t>Net Present Value ($AUD)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Average </t>
+  </si>
+  <si>
+    <t>Economic Option</t>
+  </si>
+  <si>
+    <t>Annualized Life Cycle Cost ($/kWhr)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0\ &quot;GB&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1017,7 +1027,7 @@
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1377,6 +1387,10 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="24" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -2446,8 +2460,8 @@
   </sheetPr>
   <dimension ref="A1:XFD145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3795,9 +3809,11 @@
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="118"/>
-      <c r="G57" s="118"/>
-      <c r="H57" s="118" t="s">
-        <v>133</v>
+      <c r="G57" s="125" t="s">
+        <v>186</v>
+      </c>
+      <c r="H57" s="125" t="s">
+        <v>185</v>
       </c>
       <c r="I57" s="10" t="s">
         <v>127</v>
@@ -52930,7 +52946,7 @@
     </row>
     <row r="58" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="108" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="B58" s="118">
         <v>0.1603</v>
@@ -52943,7 +52959,13 @@
       </c>
       <c r="E58" s="118"/>
       <c r="F58" s="118"/>
-      <c r="G58" s="118"/>
+      <c r="G58" s="108" t="s">
+        <v>175</v>
+      </c>
+      <c r="H58" s="126">
+        <f>AVERAGE(B58:D58)</f>
+        <v>0.17683333333333331</v>
+      </c>
     </row>
     <row r="59" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="108" t="s">
@@ -52960,7 +52982,13 @@
       </c>
       <c r="E59" s="118"/>
       <c r="F59" s="118"/>
-      <c r="G59" s="118"/>
+      <c r="G59" s="108" t="s">
+        <v>176</v>
+      </c>
+      <c r="H59" s="126">
+        <f>AVERAGE(B59:D59)</f>
+        <v>0.17910000000000001</v>
+      </c>
     </row>
     <row r="60" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="108" t="s">
@@ -52977,7 +53005,13 @@
       </c>
       <c r="E60" s="118"/>
       <c r="F60" s="118"/>
-      <c r="G60" s="118"/>
+      <c r="G60" s="108" t="s">
+        <v>177</v>
+      </c>
+      <c r="H60" s="126">
+        <f>AVERAGE(B60:D60)</f>
+        <v>0.22740000000000002</v>
+      </c>
     </row>
     <row r="61" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="108" t="s">
@@ -52994,7 +53028,13 @@
       </c>
       <c r="E61" s="118"/>
       <c r="F61" s="118"/>
-      <c r="G61" s="118"/>
+      <c r="G61" s="108" t="s">
+        <v>178</v>
+      </c>
+      <c r="H61" s="126">
+        <f>AVERAGE(B61:D61)</f>
+        <v>0.28173333333333334</v>
+      </c>
     </row>
     <row r="62" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="108" t="s">
@@ -53011,7 +53051,6 @@
       </c>
       <c r="E62" s="118"/>
       <c r="F62" s="118"/>
-      <c r="G62" s="118"/>
     </row>
     <row r="63" spans="1:16384" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="108" t="s">

</xml_diff>